<commit_message>
updated dataset for 2024 season 1-4
also created new version of Model without some of the stats
</commit_message>
<xml_diff>
--- a/Data/Prediction_Input.xlsx
+++ b/Data/Prediction_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan Chung\Desktop\NFL_Spread_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F50D20-AABE-40EA-BA1F-569E43B0D330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A32BB3-4E71-4948-8CB8-2CE88A6602CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>Dylan Chung</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{756FD02D-55E8-460F-BD99-BD30F8D8C8DE}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{FC9130F8-7505-469F-8E38-5A5F2BBA9643}">
       <text>
         <r>
           <rPr>
@@ -65,12 +65,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{5D8F68F7-0982-4526-BEB1-614FC1A85C22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dylan Chung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+this is the MARGIN of Home team, not spread</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="164">
   <si>
     <t>Week</t>
   </si>
@@ -205,12 +229,372 @@
   </si>
   <si>
     <t>Vegas_Margin</t>
+  </si>
+  <si>
+    <t>Atlanta Falcons</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers</t>
+  </si>
+  <si>
+    <t>NFC South</t>
+  </si>
+  <si>
+    <t>26.32%</t>
+  </si>
+  <si>
+    <t>42.55%</t>
+  </si>
+  <si>
+    <t>48.5</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>Atlanta Falcons4</t>
+  </si>
+  <si>
+    <t>Tampa Bay Buccaneers4</t>
+  </si>
+  <si>
+    <t>Chicago Bears</t>
+  </si>
+  <si>
+    <t>Carolina Panthers</t>
+  </si>
+  <si>
+    <t>NFC North</t>
+  </si>
+  <si>
+    <t>33.33%</t>
+  </si>
+  <si>
+    <t>29.17%</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>64.5</t>
+  </si>
+  <si>
+    <t>Chicago Bears4</t>
+  </si>
+  <si>
+    <t>Carolina Panthers4</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams</t>
+  </si>
+  <si>
+    <t>Green Bay Packers</t>
+  </si>
+  <si>
+    <t>NFC West</t>
+  </si>
+  <si>
+    <t>36.96%</t>
+  </si>
+  <si>
+    <t>40.74%</t>
+  </si>
+  <si>
+    <t>44.8</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams4</t>
+  </si>
+  <si>
+    <t>Green Bay Packers4</t>
+  </si>
+  <si>
+    <t>Cincinnati Bengals</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens</t>
+  </si>
+  <si>
+    <t>AFC North</t>
+  </si>
+  <si>
+    <t>44.68%</t>
+  </si>
+  <si>
+    <t>44.19%</t>
+  </si>
+  <si>
+    <t>36.0</t>
+  </si>
+  <si>
+    <t>89.3</t>
+  </si>
+  <si>
+    <t>Cincinnati Bengals4</t>
+  </si>
+  <si>
+    <t>Baltimore Ravens4</t>
+  </si>
+  <si>
+    <t>Houston Texans</t>
+  </si>
+  <si>
+    <t>Buffalo Bills</t>
+  </si>
+  <si>
+    <t>AFC South</t>
+  </si>
+  <si>
+    <t>AFC East</t>
+  </si>
+  <si>
+    <t>40.00%</t>
+  </si>
+  <si>
+    <t>35.71%</t>
+  </si>
+  <si>
+    <t>81.5</t>
+  </si>
+  <si>
+    <t>38.8</t>
+  </si>
+  <si>
+    <t>Houston Texans4</t>
+  </si>
+  <si>
+    <t>Buffalo Bills4</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars</t>
+  </si>
+  <si>
+    <t>Indianapolis Colts</t>
+  </si>
+  <si>
+    <t>25.00%</t>
+  </si>
+  <si>
+    <t>39.13%</t>
+  </si>
+  <si>
+    <t>53.3</t>
+  </si>
+  <si>
+    <t>39.0</t>
+  </si>
+  <si>
+    <t>Jacksonville Jaguars4</t>
+  </si>
+  <si>
+    <t>Indianapolis Colts4</t>
+  </si>
+  <si>
+    <t>San Francisco 49ers</t>
+  </si>
+  <si>
+    <t>Arizona Cardinals</t>
+  </si>
+  <si>
+    <t>43.18%</t>
+  </si>
+  <si>
+    <t>48.8</t>
+  </si>
+  <si>
+    <t>San Francisco 49ers4</t>
+  </si>
+  <si>
+    <t>Arizona Cardinals4</t>
+  </si>
+  <si>
+    <t>Denver Broncos</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders</t>
+  </si>
+  <si>
+    <t>AFC West</t>
+  </si>
+  <si>
+    <t>24.56%</t>
+  </si>
+  <si>
+    <t>32.65%</t>
+  </si>
+  <si>
+    <t>77.3</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>Denver Broncos4</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders4</t>
+  </si>
+  <si>
+    <t>New England Patriots</t>
+  </si>
+  <si>
+    <t>Miami Dolphins</t>
+  </si>
+  <si>
+    <t>32.76%</t>
+  </si>
+  <si>
+    <t>32.73%</t>
+  </si>
+  <si>
+    <t>43.0</t>
+  </si>
+  <si>
+    <t>84.0</t>
+  </si>
+  <si>
+    <t>New England Patriots4</t>
+  </si>
+  <si>
+    <t>Miami Dolphins4</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys</t>
+  </si>
+  <si>
+    <t>NFC East</t>
+  </si>
+  <si>
+    <t>43.86%</t>
+  </si>
+  <si>
+    <t>51.5</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>Pittsburgh Steelers4</t>
+  </si>
+  <si>
+    <t>Dallas Cowboys4</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks</t>
+  </si>
+  <si>
+    <t>New York Giants</t>
+  </si>
+  <si>
+    <t>39.58%</t>
+  </si>
+  <si>
+    <t>63.3</t>
+  </si>
+  <si>
+    <t>54.5</t>
+  </si>
+  <si>
+    <t>Seattle Seahawks4</t>
+  </si>
+  <si>
+    <t>New York Giants4</t>
+  </si>
+  <si>
+    <t>Washington Commanders</t>
+  </si>
+  <si>
+    <t>Cleveland Browns</t>
+  </si>
+  <si>
+    <t>53.49%</t>
+  </si>
+  <si>
+    <t>20.75%</t>
+  </si>
+  <si>
+    <t>49.3</t>
+  </si>
+  <si>
+    <t>62.5</t>
+  </si>
+  <si>
+    <t>Washington Commanders4</t>
+  </si>
+  <si>
+    <t>Cleveland Browns4</t>
+  </si>
+  <si>
+    <t>Minnesota Vikings</t>
+  </si>
+  <si>
+    <t>New York Jets</t>
+  </si>
+  <si>
+    <t>43.48%</t>
+  </si>
+  <si>
+    <t>46.30%</t>
+  </si>
+  <si>
+    <t>50.3</t>
+  </si>
+  <si>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>Minnesota Vikings4</t>
+  </si>
+  <si>
+    <t>New York Jets4</t>
+  </si>
+  <si>
+    <t>Kansas City Chiefs</t>
+  </si>
+  <si>
+    <t>New Orleans Saints</t>
+  </si>
+  <si>
+    <t>53.19%</t>
+  </si>
+  <si>
+    <t>47.5</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>Kansas City Chiefs4</t>
+  </si>
+  <si>
+    <t>New Orleans Saints4</t>
+  </si>
+  <si>
+    <t>Winner/tie</t>
+  </si>
+  <si>
+    <t>HPts</t>
+  </si>
+  <si>
+    <t>APts</t>
+  </si>
+  <si>
+    <t>Margin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -305,6 +689,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,23 +970,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:AW15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AV1" sqref="AV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,182 +1003,1595 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45568</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2">
         <v>2</v>
       </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>2024</v>
+      </c>
+      <c r="T2">
+        <v>65.86666666666666</v>
+      </c>
+      <c r="U2">
+        <v>72.45</v>
+      </c>
+      <c r="V2">
+        <v>65.3</v>
+      </c>
+      <c r="Y2">
+        <v>76.8</v>
+      </c>
+      <c r="AB2">
+        <v>71.63333333333334</v>
+      </c>
+      <c r="AC2">
+        <v>60.15</v>
+      </c>
+      <c r="AD2">
+        <v>66.8</v>
+      </c>
+      <c r="AG2">
+        <v>69</v>
+      </c>
+      <c r="AJ2">
+        <v>-10</v>
+      </c>
+      <c r="AK2">
+        <v>21</v>
+      </c>
+      <c r="AL2">
+        <v>-0.3</v>
+      </c>
+      <c r="AM2">
+        <v>0.5</v>
+      </c>
+      <c r="AN2">
+        <v>0.5</v>
+      </c>
+      <c r="AO2">
+        <v>0.75</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2024</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2024</v>
+      </c>
+      <c r="T3">
+        <v>64.2</v>
+      </c>
+      <c r="U3">
+        <v>72.45</v>
+      </c>
+      <c r="V3">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="Y3">
+        <v>64.5</v>
+      </c>
+      <c r="AB3">
+        <v>57.833333333333336</v>
+      </c>
+      <c r="AC3">
+        <v>66.5</v>
+      </c>
+      <c r="AD3">
+        <v>71.8</v>
+      </c>
+      <c r="AG3">
+        <v>73</v>
+      </c>
+      <c r="AJ3">
+        <v>2</v>
+      </c>
+      <c r="AK3">
+        <v>-56</v>
+      </c>
+      <c r="AL3">
+        <v>0.5</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0.5</v>
+      </c>
+      <c r="AO3">
+        <v>0.25</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2024</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
+      <c r="S4">
+        <v>2024</v>
+      </c>
+      <c r="T4">
+        <v>73.333333333333329</v>
+      </c>
+      <c r="U4">
+        <v>80.650000000000006</v>
+      </c>
+      <c r="V4">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="Y4">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="AB4">
+        <v>77.600000000000009</v>
+      </c>
+      <c r="AC4">
+        <v>69.5</v>
+      </c>
+      <c r="AD4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="AG4">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="AJ4">
+        <v>-40</v>
+      </c>
+      <c r="AK4">
+        <v>15</v>
+      </c>
+      <c r="AL4">
+        <v>-0.3</v>
+      </c>
+      <c r="AM4">
+        <v>1.5</v>
+      </c>
+      <c r="AN4">
+        <v>0.25</v>
+      </c>
+      <c r="AO4">
+        <v>0.5</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2024</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>2</v>
       </c>
+      <c r="S5">
+        <v>2024</v>
+      </c>
+      <c r="T5">
+        <v>70.399999999999991</v>
+      </c>
+      <c r="U5">
+        <v>66.300000000000011</v>
+      </c>
+      <c r="V5">
+        <v>88.7</v>
+      </c>
+      <c r="Y5">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="AB5">
+        <v>77.766666666666666</v>
+      </c>
+      <c r="AC5">
+        <v>79.300000000000011</v>
+      </c>
+      <c r="AD5">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="AG5">
+        <v>89.1</v>
+      </c>
+      <c r="AJ5">
+        <v>-2</v>
+      </c>
+      <c r="AK5">
+        <v>18</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0.3</v>
+      </c>
+      <c r="AN5">
+        <v>0.25</v>
+      </c>
+      <c r="AO5">
+        <v>0.5</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>2024</v>
+      </c>
+      <c r="T6">
+        <v>72.433333333333337</v>
+      </c>
+      <c r="U6">
+        <v>65.95</v>
+      </c>
+      <c r="V6">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="Y6">
+        <v>76.8</v>
+      </c>
+      <c r="AB6">
+        <v>77.166666666666671</v>
+      </c>
+      <c r="AC6">
+        <v>76.2</v>
+      </c>
+      <c r="AD6">
+        <v>71.8</v>
+      </c>
+      <c r="AG6">
+        <v>79.8</v>
+      </c>
+      <c r="AJ6">
+        <v>-15</v>
+      </c>
+      <c r="AK6">
+        <v>39</v>
+      </c>
+      <c r="AL6">
+        <v>-0.3</v>
+      </c>
+      <c r="AM6">
+        <v>1.3</v>
+      </c>
+      <c r="AN6">
+        <v>0.75</v>
+      </c>
+      <c r="AO6">
+        <v>0.75</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>87</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AV6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2024</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>2</v>
       </c>
+      <c r="S7">
+        <v>2024</v>
+      </c>
+      <c r="T7">
+        <v>69.86666666666666</v>
+      </c>
+      <c r="U7">
+        <v>58.2</v>
+      </c>
+      <c r="V7">
+        <v>85.4</v>
+      </c>
+      <c r="Y7">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="AB7">
+        <v>66.63333333333334</v>
+      </c>
+      <c r="AC7">
+        <v>70.2</v>
+      </c>
+      <c r="AD7">
+        <v>67.5</v>
+      </c>
+      <c r="AG7">
+        <v>70.8</v>
+      </c>
+      <c r="AJ7">
+        <v>-49</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>-0.5</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0.5</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AV7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2024</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8">
         <v>2</v>
       </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>2024</v>
+      </c>
+      <c r="T8">
+        <v>76.100000000000009</v>
+      </c>
+      <c r="U8">
+        <v>87.5</v>
+      </c>
+      <c r="V8">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="Y8">
+        <v>89.9</v>
+      </c>
+      <c r="AB8">
+        <v>63.433333333333337</v>
+      </c>
+      <c r="AC8">
+        <v>73.150000000000006</v>
+      </c>
+      <c r="AD8">
+        <v>84.1</v>
+      </c>
+      <c r="AG8">
+        <v>50.9</v>
+      </c>
+      <c r="AJ8">
+        <v>21</v>
+      </c>
+      <c r="AK8">
+        <v>-10</v>
+      </c>
+      <c r="AL8">
+        <v>0.5</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0.5</v>
+      </c>
+      <c r="AO8">
+        <v>0.25</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AV8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>2024</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q9">
         <v>2</v>
       </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>2024</v>
+      </c>
+      <c r="T9">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="U9">
+        <v>74.949999999999989</v>
+      </c>
+      <c r="V9">
+        <v>83.9</v>
+      </c>
+      <c r="Y9">
+        <v>60</v>
+      </c>
+      <c r="AB9">
+        <v>68.333333333333329</v>
+      </c>
+      <c r="AC9">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="AD9">
+        <v>69.8</v>
+      </c>
+      <c r="AG9">
+        <v>78.5</v>
+      </c>
+      <c r="AJ9">
+        <v>7</v>
+      </c>
+      <c r="AK9">
+        <v>-19</v>
+      </c>
+      <c r="AL9">
+        <v>-0.5</v>
+      </c>
+      <c r="AM9">
+        <v>-1</v>
+      </c>
+      <c r="AN9">
+        <v>0.5</v>
+      </c>
+      <c r="AO9">
+        <v>0.5</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV9">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>2024</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J10" t="s">
+        <v>115</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>84</v>
+      </c>
+      <c r="N10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>2024</v>
+      </c>
+      <c r="T10">
+        <v>55.966666666666661</v>
+      </c>
+      <c r="U10">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="V10">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="Y10">
+        <v>72.8</v>
+      </c>
+      <c r="AB10">
+        <v>80.966666666666669</v>
+      </c>
+      <c r="AC10">
+        <v>75.5</v>
+      </c>
+      <c r="AD10">
+        <v>66.5</v>
+      </c>
+      <c r="AG10">
+        <v>88.7</v>
+      </c>
+      <c r="AJ10">
+        <v>-35</v>
+      </c>
+      <c r="AK10">
+        <v>-58</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0.25</v>
+      </c>
+      <c r="AO10">
+        <v>0.25</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>118</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2024</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J11" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N11" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="R11">
         <v>2</v>
       </c>
+      <c r="S11">
+        <v>2024</v>
+      </c>
+      <c r="T11">
+        <v>59.79999999999999</v>
+      </c>
+      <c r="U11">
+        <v>73.3</v>
+      </c>
+      <c r="V11">
+        <v>78.3</v>
+      </c>
+      <c r="Y11">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="AB11">
+        <v>78.966666666666669</v>
+      </c>
+      <c r="AC11">
+        <v>73.300000000000011</v>
+      </c>
+      <c r="AD11">
+        <v>84.1</v>
+      </c>
+      <c r="AG11">
+        <v>87.1</v>
+      </c>
+      <c r="AJ11">
+        <v>22</v>
+      </c>
+      <c r="AK11">
+        <v>-7</v>
+      </c>
+      <c r="AL11">
+        <v>0.5</v>
+      </c>
+      <c r="AM11">
+        <v>0.3</v>
+      </c>
+      <c r="AN11">
+        <v>0.75</v>
+      </c>
+      <c r="AO11">
+        <v>0.5</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV11">
+        <v>4</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>2024</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12">
+        <v>9</v>
+      </c>
+      <c r="L12">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>65</v>
+      </c>
+      <c r="N12" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>2024</v>
+      </c>
+      <c r="T12">
+        <v>70.8</v>
+      </c>
+      <c r="U12">
+        <v>74</v>
+      </c>
+      <c r="V12">
+        <v>90.7</v>
+      </c>
+      <c r="Y12">
+        <v>73.5</v>
+      </c>
+      <c r="AB12">
+        <v>57.066666666666663</v>
+      </c>
+      <c r="AC12">
+        <v>55.2</v>
+      </c>
+      <c r="AD12">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="AG12">
+        <v>67.8</v>
+      </c>
+      <c r="AJ12">
+        <v>17</v>
+      </c>
+      <c r="AK12">
+        <v>-24</v>
+      </c>
+      <c r="AL12">
+        <v>-0.8</v>
+      </c>
+      <c r="AM12">
+        <v>-0.5</v>
+      </c>
+      <c r="AN12">
+        <v>0.75</v>
+      </c>
+      <c r="AO12">
+        <v>0.25</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AV12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2024</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13" t="s">
+        <v>124</v>
+      </c>
+      <c r="N13" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>2024</v>
+      </c>
+      <c r="T13">
+        <v>64.766666666666666</v>
+      </c>
+      <c r="U13">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="V13">
+        <v>62</v>
+      </c>
+      <c r="Y13">
+        <v>62</v>
+      </c>
+      <c r="AB13">
+        <v>62.433333333333337</v>
+      </c>
+      <c r="AC13">
+        <v>66.150000000000006</v>
+      </c>
+      <c r="AD13">
+        <v>86</v>
+      </c>
+      <c r="AG13">
+        <v>84.7</v>
+      </c>
+      <c r="AJ13">
+        <v>19</v>
+      </c>
+      <c r="AK13">
+        <v>-21</v>
+      </c>
+      <c r="AL13">
+        <v>0.3</v>
+      </c>
+      <c r="AM13">
+        <v>-0.5</v>
+      </c>
+      <c r="AN13">
+        <v>0.75</v>
+      </c>
+      <c r="AO13">
+        <v>0.25</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>139</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>141</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AV13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2024</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45571</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" t="s">
+        <v>146</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
         <v>2</v>
       </c>
+      <c r="S14">
+        <v>2024</v>
+      </c>
+      <c r="T14">
+        <v>76.466666666666683</v>
+      </c>
+      <c r="U14">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="V14">
+        <v>79</v>
+      </c>
+      <c r="Y14">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="AB14">
+        <v>53.933333333333337</v>
+      </c>
+      <c r="AC14">
+        <v>62.25</v>
+      </c>
+      <c r="AD14">
+        <v>89</v>
+      </c>
+      <c r="AG14">
+        <v>90</v>
+      </c>
+      <c r="AJ14">
+        <v>57</v>
+      </c>
+      <c r="AK14">
+        <v>14</v>
+      </c>
+      <c r="AL14">
+        <v>0.8</v>
+      </c>
+      <c r="AM14">
+        <v>0.3</v>
+      </c>
+      <c r="AN14">
+        <v>1</v>
+      </c>
+      <c r="AO14">
+        <v>0.5</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>148</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>150</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>152</v>
+      </c>
+      <c r="AV14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>2024</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45572</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="R15">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2</v>
+      <c r="S15">
+        <v>2024</v>
+      </c>
+      <c r="T15">
+        <v>74.3</v>
+      </c>
+      <c r="U15">
+        <v>71.849999999999994</v>
+      </c>
+      <c r="V15">
+        <v>90.3</v>
+      </c>
+      <c r="Y15">
+        <v>73</v>
+      </c>
+      <c r="AB15">
+        <v>68.86666666666666</v>
+      </c>
+      <c r="AC15">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="AD15">
+        <v>90.4</v>
+      </c>
+      <c r="AG15">
+        <v>77</v>
+      </c>
+      <c r="AJ15">
+        <v>20</v>
+      </c>
+      <c r="AK15">
+        <v>57</v>
+      </c>
+      <c r="AL15">
+        <v>-1</v>
+      </c>
+      <c r="AM15">
+        <v>0.8</v>
+      </c>
+      <c r="AN15">
+        <v>1</v>
+      </c>
+      <c r="AO15">
+        <v>0.5</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>157</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>158</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>159</v>
+      </c>
+      <c r="AV15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed variables, readied predictor .py
Pct Accuracy	65.02%	Accuracy >7	84.04%
at beating vegas spread
</commit_message>
<xml_diff>
--- a/Data/Prediction_Input.xlsx
+++ b/Data/Prediction_Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan Chung\Desktop\NFL_Spread_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A32BB3-4E71-4948-8CB8-2CE88A6602CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3103127-C0EA-4A59-BA70-13BF23510031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{5D8F68F7-0982-4526-BEB1-614FC1A85C22}">
+    <comment ref="AO1" authorId="0" shapeId="0" xr:uid="{5D8F68F7-0982-4526-BEB1-614FC1A85C22}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="159">
   <si>
     <t>Week</t>
   </si>
@@ -147,36 +147,12 @@
     <t>Prev_Rush</t>
   </si>
   <si>
-    <t>Prev_PPG</t>
-  </si>
-  <si>
-    <t>Prev_Sacks_Taken</t>
-  </si>
-  <si>
-    <t>Prev_Def_PPG</t>
-  </si>
-  <si>
-    <t>Def_PassRTG</t>
-  </si>
-  <si>
     <t>A_Prev_Pass</t>
   </si>
   <si>
     <t>A_Prev_Rush</t>
   </si>
   <si>
-    <t>A_Prev_PPG</t>
-  </si>
-  <si>
-    <t>A_Prev_Sacks_Taken</t>
-  </si>
-  <si>
-    <t>A_Prev_Def_PPG</t>
-  </si>
-  <si>
-    <t>A_Def_PassRTG</t>
-  </si>
-  <si>
     <t>Home_Last 5_Margin</t>
   </si>
   <si>
@@ -586,6 +562,15 @@
   </si>
   <si>
     <t>Margin</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Mon</t>
   </si>
 </sst>
 </file>
@@ -595,7 +580,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,6 +614,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -970,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW15"/>
+  <dimension ref="A1:AO15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AV1" sqref="AV1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,11 +976,9 @@
     <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,16 +992,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -1054,96 +1043,72 @@
         <v>16</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AM1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AN1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AO1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AQ1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AW1" s="4" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>2024</v>
+      <c r="B2" t="s">
+        <v>156</v>
       </c>
       <c r="C2" s="5">
         <v>45568</v>
@@ -1152,10 +1117,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K2">
         <v>7</v>
@@ -1164,10 +1129,10 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -1187,67 +1152,67 @@
       <c r="V2">
         <v>65.3</v>
       </c>
+      <c r="W2">
+        <v>76.8</v>
+      </c>
+      <c r="X2">
+        <v>71.63333333333334</v>
+      </c>
       <c r="Y2">
-        <v>76.8</v>
+        <v>60.15</v>
+      </c>
+      <c r="Z2">
+        <v>66.8</v>
+      </c>
+      <c r="AA2">
+        <v>69</v>
       </c>
       <c r="AB2">
-        <v>71.63333333333334</v>
+        <v>-10</v>
       </c>
       <c r="AC2">
-        <v>60.15</v>
+        <v>21</v>
       </c>
       <c r="AD2">
-        <v>66.8</v>
+        <v>-0.3</v>
+      </c>
+      <c r="AE2">
+        <v>0.5</v>
+      </c>
+      <c r="AF2">
+        <v>0.5</v>
       </c>
       <c r="AG2">
-        <v>69</v>
-      </c>
-      <c r="AJ2">
-        <v>-10</v>
-      </c>
-      <c r="AK2">
-        <v>21</v>
-      </c>
-      <c r="AL2">
-        <v>-0.3</v>
-      </c>
-      <c r="AM2">
-        <v>0.5</v>
+        <v>0.75</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>45</v>
       </c>
       <c r="AN2">
-        <v>0.5</v>
-      </c>
-      <c r="AO2">
-        <v>0.75</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>2024</v>
+      <c r="B3" t="s">
+        <v>157</v>
       </c>
       <c r="C3" s="5">
         <v>45571</v>
@@ -1256,10 +1221,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K3">
         <v>3</v>
@@ -1268,10 +1233,10 @@
         <v>7</v>
       </c>
       <c r="M3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="Q3">
         <v>2</v>
@@ -1291,67 +1256,67 @@
       <c r="V3">
         <v>78.599999999999994</v>
       </c>
+      <c r="W3">
+        <v>64.5</v>
+      </c>
+      <c r="X3">
+        <v>57.833333333333336</v>
+      </c>
       <c r="Y3">
-        <v>64.5</v>
+        <v>66.5</v>
+      </c>
+      <c r="Z3">
+        <v>71.8</v>
+      </c>
+      <c r="AA3">
+        <v>73</v>
       </c>
       <c r="AB3">
-        <v>57.833333333333336</v>
+        <v>2</v>
       </c>
       <c r="AC3">
-        <v>66.5</v>
+        <v>-56</v>
       </c>
       <c r="AD3">
-        <v>71.8</v>
+        <v>0.5</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0.5</v>
       </c>
       <c r="AG3">
-        <v>73</v>
-      </c>
-      <c r="AJ3">
-        <v>2</v>
-      </c>
-      <c r="AK3">
-        <v>-56</v>
-      </c>
-      <c r="AL3">
-        <v>0.5</v>
-      </c>
-      <c r="AM3">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>54</v>
       </c>
       <c r="AN3">
-        <v>0.5</v>
-      </c>
-      <c r="AO3">
-        <v>0.25</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AV3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>2024</v>
+      <c r="B4" t="s">
+        <v>157</v>
       </c>
       <c r="C4" s="5">
         <v>45571</v>
@@ -1360,10 +1325,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -1372,10 +1337,10 @@
         <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -1395,67 +1360,67 @@
       <c r="V4">
         <v>64.099999999999994</v>
       </c>
+      <c r="W4">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="X4">
+        <v>77.600000000000009</v>
+      </c>
       <c r="Y4">
-        <v>69.599999999999994</v>
+        <v>69.5</v>
+      </c>
+      <c r="Z4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="AA4">
+        <v>71.400000000000006</v>
       </c>
       <c r="AB4">
-        <v>77.600000000000009</v>
+        <v>-40</v>
       </c>
       <c r="AC4">
-        <v>69.5</v>
+        <v>15</v>
       </c>
       <c r="AD4">
-        <v>67.900000000000006</v>
+        <v>-0.3</v>
+      </c>
+      <c r="AE4">
+        <v>1.5</v>
+      </c>
+      <c r="AF4">
+        <v>0.25</v>
       </c>
       <c r="AG4">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="AJ4">
-        <v>-40</v>
-      </c>
-      <c r="AK4">
-        <v>15</v>
-      </c>
-      <c r="AL4">
-        <v>-0.3</v>
-      </c>
-      <c r="AM4">
-        <v>1.5</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>63</v>
       </c>
       <c r="AN4">
-        <v>0.25</v>
-      </c>
-      <c r="AO4">
-        <v>0.5</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AV4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>2024</v>
+      <c r="B5" t="s">
+        <v>157</v>
       </c>
       <c r="C5" s="5">
         <v>45571</v>
@@ -1464,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K5">
         <v>12</v>
@@ -1476,10 +1441,10 @@
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -1499,67 +1464,67 @@
       <c r="V5">
         <v>88.7</v>
       </c>
+      <c r="W5">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="X5">
+        <v>77.766666666666666</v>
+      </c>
       <c r="Y5">
-        <v>67.900000000000006</v>
+        <v>79.300000000000011</v>
+      </c>
+      <c r="Z5">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="AA5">
+        <v>89.1</v>
       </c>
       <c r="AB5">
-        <v>77.766666666666666</v>
+        <v>-2</v>
       </c>
       <c r="AC5">
-        <v>79.300000000000011</v>
+        <v>18</v>
       </c>
       <c r="AD5">
-        <v>79.400000000000006</v>
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0.3</v>
+      </c>
+      <c r="AF5">
+        <v>0.25</v>
       </c>
       <c r="AG5">
-        <v>89.1</v>
-      </c>
-      <c r="AJ5">
-        <v>-2</v>
-      </c>
-      <c r="AK5">
-        <v>18</v>
-      </c>
-      <c r="AL5">
-        <v>0</v>
-      </c>
-      <c r="AM5">
-        <v>0.3</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>72</v>
       </c>
       <c r="AN5">
-        <v>0.25</v>
-      </c>
-      <c r="AO5">
-        <v>0.5</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AV5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2024</v>
+      <c r="B6" t="s">
+        <v>157</v>
       </c>
       <c r="C6" s="5">
         <v>45571</v>
@@ -1568,10 +1533,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="K6">
         <v>4</v>
@@ -1580,10 +1545,10 @@
         <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="N6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="Q6">
         <v>3</v>
@@ -1603,67 +1568,67 @@
       <c r="V6">
         <v>81.099999999999994</v>
       </c>
+      <c r="W6">
+        <v>76.8</v>
+      </c>
+      <c r="X6">
+        <v>77.166666666666671</v>
+      </c>
       <c r="Y6">
-        <v>76.8</v>
+        <v>76.2</v>
+      </c>
+      <c r="Z6">
+        <v>71.8</v>
+      </c>
+      <c r="AA6">
+        <v>79.8</v>
       </c>
       <c r="AB6">
-        <v>77.166666666666671</v>
+        <v>-15</v>
       </c>
       <c r="AC6">
-        <v>76.2</v>
+        <v>39</v>
       </c>
       <c r="AD6">
-        <v>71.8</v>
+        <v>-0.3</v>
+      </c>
+      <c r="AE6">
+        <v>1.3</v>
+      </c>
+      <c r="AF6">
+        <v>0.75</v>
       </c>
       <c r="AG6">
-        <v>79.8</v>
-      </c>
-      <c r="AJ6">
-        <v>-15</v>
-      </c>
-      <c r="AK6">
-        <v>39</v>
-      </c>
-      <c r="AL6">
-        <v>-0.3</v>
-      </c>
-      <c r="AM6">
-        <v>1.3</v>
+        <v>0.75</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>82</v>
       </c>
       <c r="AN6">
-        <v>0.75</v>
-      </c>
-      <c r="AO6">
-        <v>0.75</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>2024</v>
+      <c r="B7" t="s">
+        <v>157</v>
       </c>
       <c r="C7" s="5">
         <v>45571</v>
@@ -1672,10 +1637,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K7">
         <v>9</v>
@@ -1684,10 +1649,10 @@
         <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1707,67 +1672,67 @@
       <c r="V7">
         <v>85.4</v>
       </c>
+      <c r="W7">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="X7">
+        <v>66.63333333333334</v>
+      </c>
       <c r="Y7">
-        <v>72.599999999999994</v>
+        <v>70.2</v>
+      </c>
+      <c r="Z7">
+        <v>67.5</v>
+      </c>
+      <c r="AA7">
+        <v>70.8</v>
       </c>
       <c r="AB7">
-        <v>66.63333333333334</v>
+        <v>-49</v>
       </c>
       <c r="AC7">
-        <v>70.2</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <v>67.5</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
       </c>
       <c r="AG7">
-        <v>70.8</v>
-      </c>
-      <c r="AJ7">
-        <v>-49</v>
-      </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
-      <c r="AL7">
-        <v>-0.5</v>
-      </c>
-      <c r="AM7">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>90</v>
       </c>
       <c r="AN7">
-        <v>0</v>
-      </c>
-      <c r="AO7">
-        <v>0.5</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>94</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8">
-        <v>2024</v>
+      <c r="B8" t="s">
+        <v>157</v>
       </c>
       <c r="C8" s="5">
         <v>45571</v>
@@ -1776,10 +1741,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="K8">
         <v>13</v>
@@ -1788,10 +1753,10 @@
         <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="Q8">
         <v>2</v>
@@ -1811,67 +1776,67 @@
       <c r="V8">
         <v>68.099999999999994</v>
       </c>
+      <c r="W8">
+        <v>89.9</v>
+      </c>
+      <c r="X8">
+        <v>63.433333333333337</v>
+      </c>
       <c r="Y8">
-        <v>89.9</v>
+        <v>73.150000000000006</v>
+      </c>
+      <c r="Z8">
+        <v>84.1</v>
+      </c>
+      <c r="AA8">
+        <v>50.9</v>
       </c>
       <c r="AB8">
-        <v>63.433333333333337</v>
+        <v>21</v>
       </c>
       <c r="AC8">
-        <v>73.150000000000006</v>
+        <v>-10</v>
       </c>
       <c r="AD8">
-        <v>84.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0.5</v>
       </c>
       <c r="AG8">
-        <v>50.9</v>
-      </c>
-      <c r="AJ8">
-        <v>21</v>
-      </c>
-      <c r="AK8">
-        <v>-10</v>
-      </c>
-      <c r="AL8">
-        <v>0.5</v>
-      </c>
-      <c r="AM8">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>96</v>
       </c>
       <c r="AN8">
-        <v>0.5</v>
-      </c>
-      <c r="AO8">
-        <v>0.25</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9">
-        <v>2024</v>
+      <c r="B9" t="s">
+        <v>157</v>
       </c>
       <c r="C9" s="5">
         <v>45571</v>
@@ -1880,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="K9">
         <v>5</v>
@@ -1892,10 +1857,10 @@
         <v>6</v>
       </c>
       <c r="M9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="N9" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="Q9">
         <v>2</v>
@@ -1915,67 +1880,67 @@
       <c r="V9">
         <v>83.9</v>
       </c>
+      <c r="W9">
+        <v>60</v>
+      </c>
+      <c r="X9">
+        <v>68.333333333333329</v>
+      </c>
       <c r="Y9">
-        <v>60</v>
+        <v>68.400000000000006</v>
+      </c>
+      <c r="Z9">
+        <v>69.8</v>
+      </c>
+      <c r="AA9">
+        <v>78.5</v>
       </c>
       <c r="AB9">
-        <v>68.333333333333329</v>
+        <v>7</v>
       </c>
       <c r="AC9">
-        <v>68.400000000000006</v>
+        <v>-19</v>
       </c>
       <c r="AD9">
-        <v>69.8</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AE9">
+        <v>-1</v>
+      </c>
+      <c r="AF9">
+        <v>0.5</v>
       </c>
       <c r="AG9">
-        <v>78.5</v>
-      </c>
-      <c r="AJ9">
-        <v>7</v>
-      </c>
-      <c r="AK9">
-        <v>-19</v>
-      </c>
-      <c r="AL9">
-        <v>-0.5</v>
-      </c>
-      <c r="AM9">
-        <v>-1</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>105</v>
       </c>
       <c r="AN9">
-        <v>0.5</v>
-      </c>
-      <c r="AO9">
-        <v>0.5</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>109</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>112</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>113</v>
-      </c>
-      <c r="AV9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10">
-        <v>2024</v>
+      <c r="B10" t="s">
+        <v>157</v>
       </c>
       <c r="C10" s="5">
         <v>45571</v>
@@ -1984,10 +1949,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="K10">
         <v>8</v>
@@ -1996,10 +1961,10 @@
         <v>9</v>
       </c>
       <c r="M10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="N10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -2019,67 +1984,67 @@
       <c r="V10">
         <v>77.599999999999994</v>
       </c>
+      <c r="W10">
+        <v>72.8</v>
+      </c>
+      <c r="X10">
+        <v>80.966666666666669</v>
+      </c>
       <c r="Y10">
-        <v>72.8</v>
+        <v>75.5</v>
+      </c>
+      <c r="Z10">
+        <v>66.5</v>
+      </c>
+      <c r="AA10">
+        <v>88.7</v>
       </c>
       <c r="AB10">
-        <v>80.966666666666669</v>
+        <v>-35</v>
       </c>
       <c r="AC10">
-        <v>75.5</v>
+        <v>-58</v>
       </c>
       <c r="AD10">
-        <v>66.5</v>
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0.25</v>
       </c>
       <c r="AG10">
-        <v>88.7</v>
-      </c>
-      <c r="AJ10">
-        <v>-35</v>
-      </c>
-      <c r="AK10">
-        <v>-58</v>
-      </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
-      <c r="AM10">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>113</v>
       </c>
       <c r="AN10">
-        <v>0.25</v>
-      </c>
-      <c r="AO10">
-        <v>0.25</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>118</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>119</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>121</v>
-      </c>
-      <c r="AV10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11">
-        <v>2024</v>
+      <c r="B11" t="s">
+        <v>157</v>
       </c>
       <c r="C11" s="5">
         <v>45571</v>
@@ -2088,10 +2053,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J11" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="K11">
         <v>9</v>
@@ -2100,10 +2065,10 @@
         <v>12</v>
       </c>
       <c r="M11" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="N11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="Q11">
         <v>3</v>
@@ -2123,67 +2088,67 @@
       <c r="V11">
         <v>78.3</v>
       </c>
+      <c r="W11">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="X11">
+        <v>78.966666666666669</v>
+      </c>
       <c r="Y11">
-        <v>80.900000000000006</v>
+        <v>73.300000000000011</v>
+      </c>
+      <c r="Z11">
+        <v>84.1</v>
+      </c>
+      <c r="AA11">
+        <v>87.1</v>
       </c>
       <c r="AB11">
-        <v>78.966666666666669</v>
+        <v>22</v>
       </c>
       <c r="AC11">
-        <v>73.300000000000011</v>
+        <v>-7</v>
       </c>
       <c r="AD11">
-        <v>84.1</v>
+        <v>0.5</v>
+      </c>
+      <c r="AE11">
+        <v>0.3</v>
+      </c>
+      <c r="AF11">
+        <v>0.75</v>
       </c>
       <c r="AG11">
-        <v>87.1</v>
-      </c>
-      <c r="AJ11">
-        <v>22</v>
-      </c>
-      <c r="AK11">
-        <v>-7</v>
-      </c>
-      <c r="AL11">
         <v>0.5</v>
       </c>
-      <c r="AM11">
-        <v>0.3</v>
+      <c r="AH11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>121</v>
       </c>
       <c r="AN11">
-        <v>0.75</v>
-      </c>
-      <c r="AO11">
-        <v>0.5</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>125</v>
-      </c>
-      <c r="AQ11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR11" t="s">
-        <v>126</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>128</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>129</v>
-      </c>
-      <c r="AV11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12">
-        <v>2024</v>
+      <c r="B12" t="s">
+        <v>157</v>
       </c>
       <c r="C12" s="5">
         <v>45571</v>
@@ -2192,10 +2157,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="J12" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="K12">
         <v>9</v>
@@ -2204,10 +2169,10 @@
         <v>9</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="Q12">
         <v>3</v>
@@ -2227,67 +2192,67 @@
       <c r="V12">
         <v>90.7</v>
       </c>
+      <c r="W12">
+        <v>73.5</v>
+      </c>
+      <c r="X12">
+        <v>57.066666666666663</v>
+      </c>
       <c r="Y12">
-        <v>73.5</v>
+        <v>55.2</v>
+      </c>
+      <c r="Z12">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="AA12">
+        <v>67.8</v>
       </c>
       <c r="AB12">
-        <v>57.066666666666663</v>
+        <v>17</v>
       </c>
       <c r="AC12">
-        <v>55.2</v>
+        <v>-24</v>
       </c>
       <c r="AD12">
-        <v>69.400000000000006</v>
+        <v>-0.8</v>
+      </c>
+      <c r="AE12">
+        <v>-0.5</v>
+      </c>
+      <c r="AF12">
+        <v>0.75</v>
       </c>
       <c r="AG12">
-        <v>67.8</v>
-      </c>
-      <c r="AJ12">
-        <v>17</v>
-      </c>
-      <c r="AK12">
-        <v>-24</v>
-      </c>
-      <c r="AL12">
-        <v>-0.8</v>
-      </c>
-      <c r="AM12">
-        <v>-0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>128</v>
       </c>
       <c r="AN12">
-        <v>0.75</v>
-      </c>
-      <c r="AO12">
-        <v>0.25</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>132</v>
-      </c>
-      <c r="AQ12" t="s">
-        <v>86</v>
-      </c>
-      <c r="AR12" t="s">
-        <v>133</v>
-      </c>
-      <c r="AS12" t="s">
-        <v>134</v>
-      </c>
-      <c r="AT12" t="s">
-        <v>135</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>136</v>
-      </c>
-      <c r="AV12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
-      <c r="B13">
-        <v>2024</v>
+      <c r="B13" t="s">
+        <v>157</v>
       </c>
       <c r="C13" s="5">
         <v>45571</v>
@@ -2296,10 +2261,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="J13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="K13">
         <v>9</v>
@@ -2308,10 +2273,10 @@
         <v>7</v>
       </c>
       <c r="M13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="N13" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="Q13">
         <v>3</v>
@@ -2331,67 +2296,67 @@
       <c r="V13">
         <v>62</v>
       </c>
+      <c r="W13">
+        <v>62</v>
+      </c>
+      <c r="X13">
+        <v>62.433333333333337</v>
+      </c>
       <c r="Y13">
-        <v>62</v>
+        <v>66.150000000000006</v>
+      </c>
+      <c r="Z13">
+        <v>86</v>
+      </c>
+      <c r="AA13">
+        <v>84.7</v>
       </c>
       <c r="AB13">
-        <v>62.433333333333337</v>
+        <v>19</v>
       </c>
       <c r="AC13">
-        <v>66.150000000000006</v>
+        <v>-21</v>
       </c>
       <c r="AD13">
-        <v>86</v>
+        <v>0.3</v>
+      </c>
+      <c r="AE13">
+        <v>-0.5</v>
+      </c>
+      <c r="AF13">
+        <v>0.75</v>
       </c>
       <c r="AG13">
-        <v>84.7</v>
-      </c>
-      <c r="AJ13">
-        <v>19</v>
-      </c>
-      <c r="AK13">
-        <v>-21</v>
-      </c>
-      <c r="AL13">
-        <v>0.3</v>
-      </c>
-      <c r="AM13">
-        <v>-0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>131</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AK13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL13" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>136</v>
       </c>
       <c r="AN13">
-        <v>0.75</v>
-      </c>
-      <c r="AO13">
-        <v>0.25</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>140</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>141</v>
-      </c>
-      <c r="AS13" t="s">
-        <v>142</v>
-      </c>
-      <c r="AT13" t="s">
-        <v>143</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>144</v>
-      </c>
-      <c r="AV13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>2024</v>
+      <c r="B14" t="s">
+        <v>157</v>
       </c>
       <c r="C14" s="5">
         <v>45571</v>
@@ -2400,10 +2365,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J14" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K14">
         <v>13</v>
@@ -2412,10 +2377,10 @@
         <v>7</v>
       </c>
       <c r="M14" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="N14" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="Q14">
         <v>4</v>
@@ -2435,67 +2400,67 @@
       <c r="V14">
         <v>79</v>
       </c>
+      <c r="W14">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="X14">
+        <v>53.933333333333337</v>
+      </c>
       <c r="Y14">
-        <v>68.400000000000006</v>
+        <v>62.25</v>
+      </c>
+      <c r="Z14">
+        <v>89</v>
+      </c>
+      <c r="AA14">
+        <v>90</v>
       </c>
       <c r="AB14">
-        <v>53.933333333333337</v>
+        <v>57</v>
       </c>
       <c r="AC14">
-        <v>62.25</v>
+        <v>14</v>
       </c>
       <c r="AD14">
-        <v>89</v>
+        <v>0.8</v>
+      </c>
+      <c r="AE14">
+        <v>0.3</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
       </c>
       <c r="AG14">
-        <v>90</v>
-      </c>
-      <c r="AJ14">
-        <v>57</v>
-      </c>
-      <c r="AK14">
-        <v>14</v>
-      </c>
-      <c r="AL14">
-        <v>0.8</v>
-      </c>
-      <c r="AM14">
-        <v>0.3</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>140</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>144</v>
       </c>
       <c r="AN14">
-        <v>1</v>
-      </c>
-      <c r="AO14">
-        <v>0.5</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>147</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>148</v>
-      </c>
-      <c r="AR14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>151</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>152</v>
-      </c>
-      <c r="AV14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
-      <c r="B15">
-        <v>2024</v>
+      <c r="B15" t="s">
+        <v>158</v>
       </c>
       <c r="C15" s="5">
         <v>45572</v>
@@ -2504,10 +2469,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="J15" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="K15">
         <v>14</v>
@@ -2516,10 +2481,10 @@
         <v>7</v>
       </c>
       <c r="M15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="N15" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="Q15">
         <v>4</v>
@@ -2539,62 +2504,63 @@
       <c r="V15">
         <v>90.3</v>
       </c>
+      <c r="W15">
+        <v>73</v>
+      </c>
+      <c r="X15">
+        <v>68.86666666666666</v>
+      </c>
       <c r="Y15">
-        <v>73</v>
+        <v>66.900000000000006</v>
+      </c>
+      <c r="Z15">
+        <v>90.4</v>
+      </c>
+      <c r="AA15">
+        <v>77</v>
       </c>
       <c r="AB15">
-        <v>68.86666666666666</v>
+        <v>20</v>
       </c>
       <c r="AC15">
-        <v>66.900000000000006</v>
+        <v>57</v>
       </c>
       <c r="AD15">
-        <v>90.4</v>
+        <v>-1</v>
+      </c>
+      <c r="AE15">
+        <v>0.8</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
       </c>
       <c r="AG15">
-        <v>77</v>
-      </c>
-      <c r="AJ15">
-        <v>20</v>
-      </c>
-      <c r="AK15">
-        <v>57</v>
-      </c>
-      <c r="AL15">
-        <v>-1</v>
-      </c>
-      <c r="AM15">
-        <v>0.8</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>147</v>
+      </c>
+      <c r="AJ15" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>151</v>
       </c>
       <c r="AN15">
-        <v>1</v>
-      </c>
-      <c r="AO15">
-        <v>0.5</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>49</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>155</v>
-      </c>
-      <c r="AR15" t="s">
-        <v>156</v>
-      </c>
-      <c r="AS15" t="s">
-        <v>157</v>
-      </c>
-      <c r="AT15" t="s">
-        <v>158</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>159</v>
-      </c>
-      <c r="AV15">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>